<commit_message>
9 test cases committed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CRM_TESTDATA.xlsx
+++ b/src/test/resources/testdata/CRM_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\eclipse-workspace\crmproject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9942EDD-A407-49AB-92E8-C439174F2351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE9326-01D2-4166-AE54-C5600892C55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginsuccess" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="clockoutData" sheetId="7" r:id="rId7"/>
     <sheet name="announcementData" sheetId="8" r:id="rId8"/>
     <sheet name="eventData" sheetId="9" r:id="rId9"/>
+    <sheet name="ticketData" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>username</t>
   </si>
@@ -189,6 +190,33 @@
   </si>
   <si>
     <t>dasfsg</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Lekshmi ticket</t>
+  </si>
+  <si>
+    <t>Lekshmi ticket added client abc</t>
+  </si>
+  <si>
+    <t>rfs</t>
+  </si>
+  <si>
+    <t>dfgsd</t>
+  </si>
+  <si>
+    <t>sdhdgj</t>
+  </si>
+  <si>
+    <t>tittle</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -564,6 +592,78 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BCFF631-9AE0-4A26-8ACF-BC0FCE229297}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>344</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C157F7-F08E-4117-91C4-FB54C83C3693}">
   <dimension ref="A1"/>
@@ -803,7 +903,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +972,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +1025,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94E65B3-165C-4788-B28C-0A93A550FA0B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>